<commit_message>
C3 Rev 1.1 sent to fabrication
</commit_message>
<xml_diff>
--- a/Hardware/C3-27-epaper-touch/production/C3-27-epaper-touch-all-pos.xlsx
+++ b/Hardware/C3-27-epaper-touch/production/C3-27-epaper-touch-all-pos.xlsx
@@ -112,7 +112,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
       <selection activeCell="A1" sqref="A1:E1"/>
@@ -406,13 +406,13 @@
         </is>
       </c>
       <c r="B15" s="3">
-        <v>131.40000000000001</v>
+        <v>121.98999999999999</v>
       </c>
       <c r="C15" s="3">
-        <v>-120.40000000000001</v>
+        <v>-113.2</v>
       </c>
       <c r="D15" s="3">
-        <v>-90</v>
+        <v>0</v>
       </c>
       <c r="E15" t="s">
         <v>1</v>
@@ -425,10 +425,10 @@
         </is>
       </c>
       <c r="B16" s="3">
-        <v>117.84999999999999</v>
+        <v>115.79000000000001</v>
       </c>
       <c r="C16" s="3">
-        <v>-110.2</v>
+        <v>-115.95999999999999</v>
       </c>
       <c r="D16" s="3">
         <v>180</v>
@@ -516,17 +516,17 @@
     <row r="21" spans="1:5">
       <c r="A21" t="inlineStr">
         <is>
-          <t>D1</t>
+          <t>C20</t>
         </is>
       </c>
       <c r="B21" s="3">
-        <v>154.15000000000001</v>
+        <v>123.34999999999999</v>
       </c>
       <c r="C21" s="3">
-        <v>-90.849999999999994</v>
+        <v>-80.260000000000005</v>
       </c>
       <c r="D21" s="3">
-        <v>180</v>
+        <v>-90</v>
       </c>
       <c r="E21" t="s">
         <v>1</v>
@@ -535,17 +535,17 @@
     <row r="22" spans="1:5">
       <c r="A22" t="inlineStr">
         <is>
-          <t>D2</t>
+          <t>C21</t>
         </is>
       </c>
       <c r="B22" s="3">
-        <v>156.55000000000001</v>
+        <v>123.34999999999999</v>
       </c>
       <c r="C22" s="3">
-        <v>-93.950000000000003</v>
+        <v>-88.915000000000006</v>
       </c>
       <c r="D22" s="3">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="E22" t="s">
         <v>1</v>
@@ -554,17 +554,17 @@
     <row r="23" spans="1:5">
       <c r="A23" t="inlineStr">
         <is>
-          <t>D3</t>
+          <t>D1</t>
         </is>
       </c>
       <c r="B23" s="3">
-        <v>151.65000000000001</v>
+        <v>154.15000000000001</v>
       </c>
       <c r="C23" s="3">
-        <v>-93.450000000000003</v>
+        <v>-90.849999999999994</v>
       </c>
       <c r="D23" s="3">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="E23" t="s">
         <v>1</v>
@@ -573,17 +573,17 @@
     <row r="24" spans="1:5">
       <c r="A24" t="inlineStr">
         <is>
-          <t>D4</t>
+          <t>D2</t>
         </is>
       </c>
       <c r="B24" s="3">
-        <v>137.47150099999999</v>
+        <v>156.55000000000001</v>
       </c>
       <c r="C24" s="3">
-        <v>-72.370000000000005</v>
+        <v>-93.950000000000003</v>
       </c>
       <c r="D24" s="3">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="E24" t="s">
         <v>1</v>
@@ -592,17 +592,17 @@
     <row r="25" spans="1:5">
       <c r="A25" t="inlineStr">
         <is>
-          <t>J1</t>
+          <t>D3</t>
         </is>
       </c>
       <c r="B25" s="3">
-        <v>146.34999999999999</v>
+        <v>151.65000000000001</v>
       </c>
       <c r="C25" s="3">
-        <v>-77.700000000000003</v>
+        <v>-93.450000000000003</v>
       </c>
       <c r="D25" s="3">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="E25" t="s">
         <v>1</v>
@@ -611,17 +611,17 @@
     <row r="26" spans="1:5">
       <c r="A26" t="inlineStr">
         <is>
-          <t>J2</t>
+          <t>D4</t>
         </is>
       </c>
       <c r="B26" s="3">
-        <v>124.8</v>
+        <v>137.47150099999999</v>
       </c>
       <c r="C26" s="3">
-        <v>-120.75</v>
+        <v>-72.370000000000005</v>
       </c>
       <c r="D26" s="3">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="E26" t="s">
         <v>1</v>
@@ -630,17 +630,17 @@
     <row r="27" spans="1:5">
       <c r="A27" t="inlineStr">
         <is>
-          <t>J4</t>
+          <t>D5</t>
         </is>
       </c>
       <c r="B27" s="3">
-        <v>119.40000000000001</v>
+        <v>117.48</v>
       </c>
       <c r="C27" s="3">
-        <v>-89</v>
+        <v>-108.95999999999999</v>
       </c>
       <c r="D27" s="3">
-        <v>180</v>
+        <v>-90</v>
       </c>
       <c r="E27" t="s">
         <v>1</v>
@@ -649,17 +649,17 @@
     <row r="28" spans="1:5">
       <c r="A28" t="inlineStr">
         <is>
-          <t>JP1</t>
+          <t>J1</t>
         </is>
       </c>
       <c r="B28" s="3">
-        <v>130.34999999999999</v>
+        <v>146.34999999999999</v>
       </c>
       <c r="C28" s="3">
-        <v>-94.530000000000001</v>
+        <v>-77.700000000000003</v>
       </c>
       <c r="D28" s="3">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="E28" t="s">
         <v>1</v>
@@ -668,17 +668,17 @@
     <row r="29" spans="1:5">
       <c r="A29" t="inlineStr">
         <is>
-          <t>L1</t>
+          <t>J2</t>
         </is>
       </c>
       <c r="B29" s="3">
-        <v>156.65000000000001</v>
+        <v>124.8</v>
       </c>
       <c r="C29" s="3">
-        <v>-98.049999999999997</v>
+        <v>-120.75</v>
       </c>
       <c r="D29" s="3">
-        <v>-90</v>
+        <v>0</v>
       </c>
       <c r="E29" t="s">
         <v>1</v>
@@ -687,17 +687,17 @@
     <row r="30" spans="1:5">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Q1</t>
+          <t>J4</t>
         </is>
       </c>
       <c r="B30" s="3">
-        <v>138.65000000000001</v>
+        <v>119.40000000000001</v>
       </c>
       <c r="C30" s="3">
-        <v>-86.5</v>
+        <v>-89</v>
       </c>
       <c r="D30" s="3">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="E30" t="s">
         <v>1</v>
@@ -706,17 +706,17 @@
     <row r="31" spans="1:5">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Q2</t>
+          <t>JP1</t>
         </is>
       </c>
       <c r="B31" s="3">
-        <v>154.65000000000001</v>
+        <v>130.34999999999999</v>
       </c>
       <c r="C31" s="3">
-        <v>-119.84999999999999</v>
+        <v>-94.530000000000001</v>
       </c>
       <c r="D31" s="3">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="E31" t="s">
         <v>1</v>
@@ -725,17 +725,17 @@
     <row r="32" spans="1:5">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Q3</t>
+          <t>L1</t>
         </is>
       </c>
       <c r="B32" s="3">
-        <v>149.30000000000001</v>
+        <v>156.65000000000001</v>
       </c>
       <c r="C32" s="3">
-        <v>-102.23999999999999</v>
+        <v>-98.049999999999997</v>
       </c>
       <c r="D32" s="3">
-        <v>180</v>
+        <v>-90</v>
       </c>
       <c r="E32" t="s">
         <v>1</v>
@@ -744,17 +744,17 @@
     <row r="33" spans="1:5">
       <c r="A33" t="inlineStr">
         <is>
-          <t>R1</t>
+          <t>Q1</t>
         </is>
       </c>
       <c r="B33" s="3">
-        <v>134.90000000000001</v>
+        <v>138.65000000000001</v>
       </c>
       <c r="C33" s="3">
-        <v>-85.849999999999994</v>
+        <v>-86.5</v>
       </c>
       <c r="D33" s="3">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="E33" t="s">
         <v>1</v>
@@ -763,14 +763,14 @@
     <row r="34" spans="1:5">
       <c r="A34" t="inlineStr">
         <is>
-          <t>R2</t>
+          <t>Q2</t>
         </is>
       </c>
       <c r="B34" s="3">
-        <v>158.155</v>
+        <v>154.65000000000001</v>
       </c>
       <c r="C34" s="3">
-        <v>-120.81999999999999</v>
+        <v>-119.84999999999999</v>
       </c>
       <c r="D34" s="3">
         <v>180</v>
@@ -782,17 +782,17 @@
     <row r="35" spans="1:5">
       <c r="A35" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>Q3</t>
         </is>
       </c>
       <c r="B35" s="3">
-        <v>135.30000000000001</v>
+        <v>149.30000000000001</v>
       </c>
       <c r="C35" s="3">
-        <v>-89.530000000000001</v>
+        <v>-102.23999999999999</v>
       </c>
       <c r="D35" s="3">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="E35" t="s">
         <v>1</v>
@@ -801,17 +801,17 @@
     <row r="36" spans="1:5">
       <c r="A36" t="inlineStr">
         <is>
-          <t>R4</t>
+          <t>R1</t>
         </is>
       </c>
       <c r="B36" s="3">
-        <v>158.91</v>
+        <v>134.90000000000001</v>
       </c>
       <c r="C36" s="3">
-        <v>-118.48999999999999</v>
+        <v>-85.849999999999994</v>
       </c>
       <c r="D36" s="3">
-        <v>-90</v>
+        <v>180</v>
       </c>
       <c r="E36" t="s">
         <v>1</v>
@@ -820,14 +820,14 @@
     <row r="37" spans="1:5">
       <c r="A37" t="inlineStr">
         <is>
-          <t>R5</t>
+          <t>R2</t>
         </is>
       </c>
       <c r="B37" s="3">
-        <v>152.91999999999999</v>
+        <v>158.155</v>
       </c>
       <c r="C37" s="3">
-        <v>-103.20999999999999</v>
+        <v>-120.81999999999999</v>
       </c>
       <c r="D37" s="3">
         <v>180</v>
@@ -839,17 +839,17 @@
     <row r="38" spans="1:5">
       <c r="A38" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="B38" s="3">
-        <v>117.65000000000001</v>
+        <v>135.30000000000001</v>
       </c>
       <c r="C38" s="3">
-        <v>-120.75</v>
+        <v>-89.530000000000001</v>
       </c>
       <c r="D38" s="3">
-        <v>-90</v>
+        <v>0</v>
       </c>
       <c r="E38" t="s">
         <v>1</v>
@@ -858,17 +858,17 @@
     <row r="39" spans="1:5">
       <c r="A39" t="inlineStr">
         <is>
-          <t>R7</t>
+          <t>R4</t>
         </is>
       </c>
       <c r="B39" s="3">
-        <v>127.5</v>
+        <v>158.91</v>
       </c>
       <c r="C39" s="3">
-        <v>-114.09999999999999</v>
+        <v>-118.48999999999999</v>
       </c>
       <c r="D39" s="3">
-        <v>0</v>
+        <v>-90</v>
       </c>
       <c r="E39" t="s">
         <v>1</v>
@@ -877,17 +877,17 @@
     <row r="40" spans="1:5">
       <c r="A40" t="inlineStr">
         <is>
-          <t>R8</t>
+          <t>R5</t>
         </is>
       </c>
       <c r="B40" s="3">
-        <v>155</v>
+        <v>152.91999999999999</v>
       </c>
       <c r="C40" s="3">
-        <v>-115.84999999999999</v>
+        <v>-103.20999999999999</v>
       </c>
       <c r="D40" s="3">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="E40" t="s">
         <v>1</v>
@@ -896,17 +896,17 @@
     <row r="41" spans="1:5">
       <c r="A41" t="inlineStr">
         <is>
-          <t>R9</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="B41" s="3">
-        <v>121.02500000000001</v>
+        <v>117.65000000000001</v>
       </c>
       <c r="C41" s="3">
-        <v>-95.819999999999993</v>
+        <v>-120.75</v>
       </c>
       <c r="D41" s="3">
-        <v>0</v>
+        <v>-90</v>
       </c>
       <c r="E41" t="s">
         <v>1</v>
@@ -915,17 +915,17 @@
     <row r="42" spans="1:5">
       <c r="A42" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>R7</t>
         </is>
       </c>
       <c r="B42" s="3">
-        <v>118.825</v>
+        <v>127.5</v>
       </c>
       <c r="C42" s="3">
-        <v>-94.200000000000003</v>
+        <v>-114.09999999999999</v>
       </c>
       <c r="D42" s="3">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="E42" t="s">
         <v>1</v>
@@ -934,17 +934,17 @@
     <row r="43" spans="1:5">
       <c r="A43" t="inlineStr">
         <is>
-          <t>R11</t>
+          <t>R8</t>
         </is>
       </c>
       <c r="B43" s="3">
-        <v>128.94999999999999</v>
+        <v>155</v>
       </c>
       <c r="C43" s="3">
-        <v>-90.549999999999997</v>
+        <v>-115.84999999999999</v>
       </c>
       <c r="D43" s="3">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="E43" t="s">
         <v>1</v>
@@ -953,17 +953,17 @@
     <row r="44" spans="1:5">
       <c r="A44" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>R9</t>
         </is>
       </c>
       <c r="B44" s="3">
-        <v>123.15000000000001</v>
+        <v>121.02500000000001</v>
       </c>
       <c r="C44" s="3">
-        <v>-88.349999999999994</v>
+        <v>-95.819999999999993</v>
       </c>
       <c r="D44" s="3">
-        <v>-90</v>
+        <v>0</v>
       </c>
       <c r="E44" t="s">
         <v>1</v>
@@ -972,17 +972,17 @@
     <row r="45" spans="1:5">
       <c r="A45" t="inlineStr">
         <is>
-          <t>R13</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="B45" s="3">
-        <v>129.50999999999999</v>
+        <v>118.825</v>
       </c>
       <c r="C45" s="3">
-        <v>-107.3</v>
+        <v>-94.200000000000003</v>
       </c>
       <c r="D45" s="3">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="E45" t="s">
         <v>1</v>
@@ -991,14 +991,14 @@
     <row r="46" spans="1:5">
       <c r="A46" t="inlineStr">
         <is>
-          <t>R14</t>
+          <t>R11</t>
         </is>
       </c>
       <c r="B46" s="3">
-        <v>129.47999999999999</v>
+        <v>128.94999999999999</v>
       </c>
       <c r="C46" s="3">
-        <v>-105.22</v>
+        <v>-90.549999999999997</v>
       </c>
       <c r="D46" s="3">
         <v>0</v>
@@ -1010,14 +1010,14 @@
     <row r="47" spans="1:5">
       <c r="A47" t="inlineStr">
         <is>
-          <t>R15</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="B47" s="3">
-        <v>129.25999999999999</v>
+        <v>120.01000000000001</v>
       </c>
       <c r="C47" s="3">
-        <v>-103.92</v>
+        <v>-98.180000000000007</v>
       </c>
       <c r="D47" s="3">
         <v>-90</v>
@@ -1029,14 +1029,14 @@
     <row r="48" spans="1:5">
       <c r="A48" t="inlineStr">
         <is>
-          <t>U2</t>
+          <t>R13</t>
         </is>
       </c>
       <c r="B48" s="3">
-        <v>125.15000000000001</v>
+        <v>129.50999999999999</v>
       </c>
       <c r="C48" s="3">
-        <v>-105.72499999999999</v>
+        <v>-107.3</v>
       </c>
       <c r="D48" s="3">
         <v>90</v>
@@ -1048,17 +1048,17 @@
     <row r="49" spans="1:5">
       <c r="A49" t="inlineStr">
         <is>
-          <t>U3</t>
+          <t>R14</t>
         </is>
       </c>
       <c r="B49" s="3">
-        <v>121.7</v>
+        <v>129.47999999999999</v>
       </c>
       <c r="C49" s="3">
-        <v>-113.0625</v>
+        <v>-105.22</v>
       </c>
       <c r="D49" s="3">
-        <v>-90</v>
+        <v>0</v>
       </c>
       <c r="E49" t="s">
         <v>1</v>
@@ -1067,19 +1067,95 @@
     <row r="50" spans="1:5">
       <c r="A50" t="inlineStr">
         <is>
+          <t>R15</t>
+        </is>
+      </c>
+      <c r="B50" s="3">
+        <v>129.25999999999999</v>
+      </c>
+      <c r="C50" s="3">
+        <v>-103.92</v>
+      </c>
+      <c r="D50" s="3">
+        <v>-90</v>
+      </c>
+      <c r="E50" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>U2</t>
+        </is>
+      </c>
+      <c r="B51" s="3">
+        <v>125.15000000000001</v>
+      </c>
+      <c r="C51" s="3">
+        <v>-105.72499999999999</v>
+      </c>
+      <c r="D51" s="3">
+        <v>90</v>
+      </c>
+      <c r="E51" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>U3</t>
+        </is>
+      </c>
+      <c r="B52" s="3">
+        <v>118.05</v>
+      </c>
+      <c r="C52" s="3">
+        <v>-113.19</v>
+      </c>
+      <c r="D52" s="3">
+        <v>0</v>
+      </c>
+      <c r="E52" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" t="inlineStr">
+        <is>
           <t>U4</t>
         </is>
       </c>
-      <c r="B50" s="3">
-        <v>127.84999999999999</v>
-      </c>
-      <c r="C50" s="3">
-        <v>-85.5</v>
-      </c>
-      <c r="D50" s="3">
-        <v>0</v>
-      </c>
-      <c r="E50" t="s">
+      <c r="B53" s="3">
+        <v>128.66</v>
+      </c>
+      <c r="C53" s="3">
+        <v>-84.989999999999995</v>
+      </c>
+      <c r="D53" s="3">
+        <v>0</v>
+      </c>
+      <c r="E53" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Y1</t>
+        </is>
+      </c>
+      <c r="B54" s="3">
+        <v>123.34999999999999</v>
+      </c>
+      <c r="C54" s="3">
+        <v>-84.159999999999997</v>
+      </c>
+      <c r="D54" s="3">
+        <v>90</v>
+      </c>
+      <c r="E54" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>